<commit_message>
added error conditions specific to shallowDoc in excelParser
</commit_message>
<xml_diff>
--- a/Schablonen/Diagnose_Intensivlungenthorax.xlsx
+++ b/Schablonen/Diagnose_Intensivlungenthorax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\radiospeech\Schablonen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCC1924B-1426-4EAA-A3CB-1EE8DA2C805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E61C82F-BB61-47A8-AEF7-DFC2E0F9EED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61320" yWindow="6690" windowWidth="29040" windowHeight="15720" xr2:uid="{572D8DC6-BB5E-46AD-A505-01D3F4CF4928}"/>
+    <workbookView xWindow="-29445" yWindow="3960" windowWidth="28620" windowHeight="13680" xr2:uid="{572D8DC6-BB5E-46AD-A505-01D3F4CF4928}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Gliederung</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Freie abdominelle Luft</t>
+  </si>
+  <si>
+    <t>Variable-Default</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -251,11 +254,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -269,9 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -287,7 +302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -583,31 +598,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF998FC-F43A-442C-BC88-4E18A442F10B}">
-  <dimension ref="A1:O88"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" customWidth="1"/>
-    <col min="4" max="4" width="115.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="115.7109375" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="2.1796875" customWidth="1"/>
-    <col min="7" max="7" width="3.26953125" customWidth="1"/>
-    <col min="8" max="9" width="3" customWidth="1"/>
-    <col min="10" max="10" width="3.54296875" customWidth="1"/>
-    <col min="11" max="11" width="3.7265625" customWidth="1"/>
-    <col min="12" max="12" width="2.7265625" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" customWidth="1"/>
+    <col min="7" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,16 +660,19 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -678,8 +696,9 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
@@ -699,8 +718,9 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
@@ -720,8 +740,9 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
@@ -741,8 +762,9 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
@@ -762,8 +784,9 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
@@ -783,8 +806,9 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
@@ -804,8 +828,9 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
@@ -825,8 +850,9 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
@@ -846,8 +872,9 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -863,8 +890,9 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -880,8 +908,9 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -897,8 +926,9 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -914,8 +944,9 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -931,8 +962,9 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -948,8 +980,9 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -965,8 +998,9 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -982,8 +1016,9 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -999,8 +1034,9 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1016,8 +1052,9 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1033,8 +1070,9 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1050,8 +1088,9 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1067,8 +1106,9 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1084,8 +1124,9 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1101,8 +1142,9 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1118,8 +1160,9 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1135,8 +1178,9 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1152,8 +1196,9 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1169,8 +1214,9 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1186,8 +1232,9 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1203,8 +1250,9 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-    </row>
-    <row r="32" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1220,8 +1268,9 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-    </row>
-    <row r="33" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1237,8 +1286,9 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-    </row>
-    <row r="34" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1254,8 +1304,9 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-    </row>
-    <row r="35" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1271,8 +1322,9 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-    </row>
-    <row r="36" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1288,8 +1340,9 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-    </row>
-    <row r="37" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1305,8 +1358,9 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-    </row>
-    <row r="38" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1322,8 +1376,9 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-    </row>
-    <row r="39" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1339,8 +1394,9 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1356,8 +1412,9 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-    </row>
-    <row r="41" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1373,8 +1430,9 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
-    </row>
-    <row r="42" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1390,8 +1448,9 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-    </row>
-    <row r="43" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P42" s="2"/>
+    </row>
+    <row r="43" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1407,8 +1466,9 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
-    </row>
-    <row r="44" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1424,8 +1484,9 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-    </row>
-    <row r="45" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1441,8 +1502,9 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
-    </row>
-    <row r="46" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P45" s="2"/>
+    </row>
+    <row r="46" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1458,8 +1520,9 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
-    </row>
-    <row r="47" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P46" s="2"/>
+    </row>
+    <row r="47" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1475,8 +1538,9 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
-    </row>
-    <row r="48" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1492,8 +1556,9 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
-    </row>
-    <row r="49" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1507,10 +1572,11 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="2"/>
-    </row>
-    <row r="50" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N49" s="2"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="2"/>
+    </row>
+    <row r="50" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1524,9 +1590,10 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="5"/>
-      <c r="O50" s="6"/>
-    </row>
-    <row r="51" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N50" s="5"/>
+      <c r="P50" s="6"/>
+    </row>
+    <row r="51" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1539,11 +1606,12 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="2"/>
-    </row>
-    <row r="52" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M51" s="4"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="2"/>
+    </row>
+    <row r="52" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1555,10 +1623,10 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="5"/>
-      <c r="M52" s="8"/>
-      <c r="O52" s="6"/>
-    </row>
-    <row r="53" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N52" s="8"/>
+      <c r="P52" s="6"/>
+    </row>
+    <row r="53" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1571,10 +1639,11 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="9"/>
-      <c r="M53" s="5"/>
-      <c r="O53" s="6"/>
-    </row>
-    <row r="54" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M53" s="11"/>
+      <c r="N53" s="5"/>
+      <c r="P53" s="6"/>
+    </row>
+    <row r="54" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1588,9 +1657,10 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="5"/>
-      <c r="O54" s="6"/>
-    </row>
-    <row r="55" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N54" s="5"/>
+      <c r="P54" s="6"/>
+    </row>
+    <row r="55" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1604,9 +1674,10 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="5"/>
-      <c r="O55" s="6"/>
-    </row>
-    <row r="56" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N55" s="5"/>
+      <c r="P55" s="6"/>
+    </row>
+    <row r="56" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1620,9 +1691,10 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="5"/>
-      <c r="O56" s="6"/>
-    </row>
-    <row r="57" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N56" s="5"/>
+      <c r="P56" s="6"/>
+    </row>
+    <row r="57" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1636,10 +1708,11 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
-      <c r="N57" s="9"/>
-      <c r="O57" s="2"/>
-    </row>
-    <row r="58" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N57" s="2"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="2"/>
+    </row>
+    <row r="58" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1655,8 +1728,9 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
-    </row>
-    <row r="59" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P58" s="2"/>
+    </row>
+    <row r="59" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1672,8 +1746,9 @@
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
-    </row>
-    <row r="60" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1689,8 +1764,9 @@
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
-    </row>
-    <row r="61" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P60" s="2"/>
+    </row>
+    <row r="61" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1706,8 +1782,9 @@
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
-    </row>
-    <row r="62" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P61" s="2"/>
+    </row>
+    <row r="62" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1723,8 +1800,9 @@
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
-    </row>
-    <row r="63" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P62" s="2"/>
+    </row>
+    <row r="63" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1740,8 +1818,9 @@
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
-    </row>
-    <row r="64" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P63" s="2"/>
+    </row>
+    <row r="64" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1757,8 +1836,9 @@
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
-    </row>
-    <row r="65" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P64" s="2"/>
+    </row>
+    <row r="65" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1774,8 +1854,9 @@
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
-    </row>
-    <row r="66" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P65" s="2"/>
+    </row>
+    <row r="66" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1791,8 +1872,9 @@
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
-    </row>
-    <row r="67" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P66" s="2"/>
+    </row>
+    <row r="67" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1808,8 +1890,9 @@
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
-    </row>
-    <row r="68" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P67" s="2"/>
+    </row>
+    <row r="68" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1825,8 +1908,9 @@
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
-    </row>
-    <row r="69" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1842,8 +1926,9 @@
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
-    </row>
-    <row r="70" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P69" s="2"/>
+    </row>
+    <row r="70" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1859,8 +1944,9 @@
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
-    </row>
-    <row r="71" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P70" s="2"/>
+    </row>
+    <row r="71" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1876,8 +1962,9 @@
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
-    </row>
-    <row r="72" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P71" s="2"/>
+    </row>
+    <row r="72" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -1893,8 +1980,9 @@
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
-    </row>
-    <row r="73" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P72" s="2"/>
+    </row>
+    <row r="73" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1910,8 +1998,9 @@
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
-    </row>
-    <row r="74" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P73" s="2"/>
+    </row>
+    <row r="74" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1927,8 +2016,9 @@
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
-    </row>
-    <row r="75" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P74" s="2"/>
+    </row>
+    <row r="75" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -1944,8 +2034,9 @@
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
-    </row>
-    <row r="76" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P75" s="2"/>
+    </row>
+    <row r="76" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1961,8 +2052,9 @@
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
-    </row>
-    <row r="77" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P76" s="2"/>
+    </row>
+    <row r="77" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1978,8 +2070,9 @@
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
-    </row>
-    <row r="78" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P77" s="2"/>
+    </row>
+    <row r="78" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1995,8 +2088,9 @@
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
-    </row>
-    <row r="79" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P78" s="2"/>
+    </row>
+    <row r="79" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2012,8 +2106,9 @@
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
-    </row>
-    <row r="80" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P79" s="2"/>
+    </row>
+    <row r="80" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2029,8 +2124,9 @@
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
-    </row>
-    <row r="81" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P80" s="2"/>
+    </row>
+    <row r="81" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2046,8 +2142,9 @@
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
-    </row>
-    <row r="82" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P81" s="2"/>
+    </row>
+    <row r="82" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2063,8 +2160,9 @@
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
-    </row>
-    <row r="83" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P82" s="2"/>
+    </row>
+    <row r="83" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2080,8 +2178,9 @@
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
-    </row>
-    <row r="84" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P83" s="2"/>
+    </row>
+    <row r="84" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2097,8 +2196,9 @@
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
-    </row>
-    <row r="85" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P84" s="2"/>
+    </row>
+    <row r="85" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2114,8 +2214,9 @@
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
-    </row>
-    <row r="86" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P85" s="2"/>
+    </row>
+    <row r="86" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2131,8 +2232,9 @@
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
-    </row>
-    <row r="87" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P86" s="2"/>
+    </row>
+    <row r="87" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2148,8 +2250,9 @@
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
-    </row>
-    <row r="88" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P87" s="2"/>
+    </row>
+    <row r="88" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2165,6 +2268,7 @@
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
+      <c r="P88" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>